<commit_message>
updated addresses in excel
</commit_message>
<xml_diff>
--- a/pipeline register info.xlsx
+++ b/pipeline register info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandralday/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gyaanantia/Desktop/pipeline_proc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CD4E19-AF71-0343-A2DA-4BA07F3FCAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B129067-545D-B54D-8ED3-9AB6F703053F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19600" yWindow="1440" windowWidth="18300" windowHeight="17440" xr2:uid="{B30A0E21-0B5A-1844-87E0-C0CEF66D9D03}"/>
+    <workbookView xWindow="8740" yWindow="1260" windowWidth="18300" windowHeight="17440" xr2:uid="{B30A0E21-0B5A-1844-87E0-C0CEF66D9D03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="77">
   <si>
     <t>Description</t>
   </si>
@@ -190,6 +190,81 @@
   </si>
   <si>
     <t>selected lower-bit instruction</t>
+  </si>
+  <si>
+    <t>Actual Wire name</t>
+  </si>
+  <si>
+    <t>ifid_out[15:11]</t>
+  </si>
+  <si>
+    <t>ifid_out[10:16]</t>
+  </si>
+  <si>
+    <t>ext_out</t>
+  </si>
+  <si>
+    <t>ifid_out[63:32]</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>RegWrite</t>
+  </si>
+  <si>
+    <t>ALUSrc</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>MemWrite</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>ALUOp</t>
+  </si>
+  <si>
+    <t>142:141</t>
+  </si>
+  <si>
+    <t>MemtoReg</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>MemRead</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>Bgtz</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>Bne</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>Beq</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>RegDst</t>
+  </si>
+  <si>
+    <t>148</t>
   </si>
 </sst>
 </file>
@@ -233,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -247,6 +322,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,28 +640,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA7966-9EE7-3240-BCEC-A7F545B97576}">
-  <dimension ref="A2:F26"/>
+  <dimension ref="A2:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="22.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -596,12 +674,15 @@
       <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -613,12 +694,12 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -628,261 +709,244 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="E6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="E7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" t="s">
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" t="s">
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C9">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C16">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="C10">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C17">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" t="s">
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="C11">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C18">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c r="C12">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C19">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" t="s">
         <v>47</v>
       </c>
-      <c r="C13">
+      <c r="C20">
         <v>5</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D20" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+      <c r="B21" t="s">
         <v>48</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17">
-        <v>32</v>
-      </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19">
-        <v>32</v>
-      </c>
-      <c r="D19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20">
-        <v>32</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" t="s">
-        <v>51</v>
       </c>
       <c r="C21">
         <v>5</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>14</v>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B22" t="s">
         <v>16</v>
@@ -890,67 +954,181 @@
       <c r="C22" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
       <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27">
+        <v>32</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+      <c r="B30" t="s">
         <v>44</v>
       </c>
-      <c r="C23">
-        <v>32</v>
-      </c>
-      <c r="D23" s="7" t="s">
+      <c r="C30">
+        <v>32</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E30" s="7"/>
+      <c r="F30" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+      <c r="B31" t="s">
         <v>29</v>
       </c>
-      <c r="C24">
-        <v>32</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="C31">
+        <v>32</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E31" s="6"/>
+      <c r="F31" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" t="s">
         <v>51</v>
       </c>
-      <c r="C25">
+      <c r="C32">
         <v>5</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D26" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A6:A14"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A8:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>